<commit_message>
Unimplemented standard functions shouldn't throw exceptions, but return #NAME? (just like UDF do). That is more in-line with behavior of opening excel with a function from new version of Excel in old excel. CalcEngine shouldn't throw exceptions, unless there is an internal bug. Unimplemented function is not internal bug.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Misc/FormulasWithEvaluation.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Misc/FormulasWithEvaluation.xlsx
@@ -558,11 +558,13 @@
         <x:f t="array" ref="B6:B6">A2+A3</x:f>
         <x:v>2</x:v>
       </x:c>
-      <x:c r="C6" s="0">
+      <x:c r="C6" s="0" t="e">
         <x:f t="array" ref="C6:D6">TRANSPOSE(A2:A3)</x:f>
-      </x:c>
-      <x:c r="D6" s="0">
+        <x:v>#NAME?</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="e">
         <x:f t="array"/>
+        <x:v>#NAME?</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:7">

</xml_diff>